<commit_message>
fix small issues in model scripts
</commit_message>
<xml_diff>
--- a/data/population_models/models_output_kriegberg.xlsx
+++ b/data/population_models/models_output_kriegberg.xlsx
@@ -422,7 +422,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -432,23 +432,23 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~1)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~1)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F2">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>286.7557688343559</v>
+        <v>87.04659848148148</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.2113503148468601</v>
+        <v>0.3330270270279794</v>
       </c>
       <c r="J2">
-        <v>-525.57242</v>
+        <v>-41.443963</v>
       </c>
     </row>
     <row r="3">
@@ -459,12 +459,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -474,23 +474,23 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~temp)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>287.2959025925926</v>
+        <v>87.1192323076923</v>
       </c>
       <c r="H3">
-        <v>0.5401337582367205</v>
+        <v>0.0726338262108186</v>
       </c>
       <c r="I3">
-        <v>0.1613297065263859</v>
+        <v>0.3211494964769983</v>
       </c>
       <c r="J3">
-        <v>-527.39175</v>
+        <v>-44.19754</v>
       </c>
     </row>
     <row r="4">
@@ -501,7 +501,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -516,34 +516,34 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~time)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>287.6382325925926</v>
+        <v>89.86769930769231</v>
       </c>
       <c r="H4">
-        <v>0.8824637582367245</v>
+        <v>2.821100826210824</v>
       </c>
       <c r="I4">
-        <v>0.1359497235471803</v>
+        <v>0.08126157201169604</v>
       </c>
       <c r="J4">
-        <v>-527.0494200000001</v>
+        <v>-41.449073</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -558,23 +558,23 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F5">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>287.76401</v>
+        <v>89.87052730769231</v>
       </c>
       <c r="H5">
-        <v>1.008241165644108</v>
+        <v>2.823928826210832</v>
       </c>
       <c r="I5">
-        <v>0.1276633133377709</v>
+        <v>0.081146749347626</v>
       </c>
       <c r="J5">
-        <v>-531.73105</v>
+        <v>-41.446245</v>
       </c>
     </row>
     <row r="6">
@@ -585,12 +585,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -600,23 +600,23 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~wind)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F6">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>289.0913525925926</v>
+        <v>89.94076099999999</v>
       </c>
       <c r="H6">
-        <v>2.335583758236737</v>
+        <v>2.894162518518513</v>
       </c>
       <c r="I6">
-        <v>0.06574115501930779</v>
+        <v>0.07834658564970837</v>
       </c>
       <c r="J6">
-        <v>-525.59629</v>
+        <v>-44.428319</v>
       </c>
     </row>
     <row r="7">
@@ -627,12 +627,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -642,29 +642,29 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~temp + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F7">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>289.1421325925926</v>
+        <v>90.13548400000001</v>
       </c>
       <c r="H7">
-        <v>2.386363758236712</v>
+        <v>3.088885518518524</v>
       </c>
       <c r="I7">
-        <v>0.06409299897401671</v>
+        <v>0.07107821494683383</v>
       </c>
       <c r="J7">
-        <v>-525.54552</v>
+        <v>-44.233596</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -684,23 +684,23 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur + wind)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~sundur + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G8">
-        <v>289.4675464596273</v>
+        <v>92.917738</v>
       </c>
       <c r="H8">
-        <v>2.711777625271452</v>
+        <v>5.871139518518518</v>
       </c>
       <c r="I8">
-        <v>0.05446880781042903</v>
+        <v>0.01768388706520641</v>
       </c>
       <c r="J8">
-        <v>-527.60888</v>
+        <v>-41.451341</v>
       </c>
     </row>
     <row r="9">
@@ -711,12 +711,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -726,23 +726,23 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F9">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>289.6367164596273</v>
+        <v>93.15929966666667</v>
       </c>
       <c r="H9">
-        <v>2.88094762527146</v>
+        <v>6.112701185185188</v>
       </c>
       <c r="I9">
-        <v>0.05005103596108108</v>
+        <v>0.01567195887199801</v>
       </c>
       <c r="J9">
-        <v>-527.43971</v>
+        <v>-44.516446</v>
       </c>
     </row>
     <row r="10">
@@ -753,7 +753,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -768,39 +768,39 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur + wind)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~1)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F10">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G10">
-        <v>289.6683864596274</v>
+        <v>100.514298</v>
       </c>
       <c r="H10">
-        <v>2.91261762527148</v>
+        <v>13.46769951851851</v>
       </c>
       <c r="I10">
-        <v>0.04926471989457243</v>
+        <v>0.0003962832243656278</v>
       </c>
       <c r="J10">
-        <v>-527.40804</v>
+        <v>-53.694782</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -810,29 +810,29 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~1)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F11">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G11">
-        <v>291.5034764596273</v>
+        <v>104.21149</v>
       </c>
       <c r="H11">
-        <v>4.74770762527146</v>
+        <v>17.16489151851852</v>
       </c>
       <c r="I11">
-        <v>0.01968118698473208</v>
+        <v>6.239799657287439E-05</v>
       </c>
       <c r="J11">
-        <v>-525.57294</v>
+        <v>-49.997589</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -852,23 +852,23 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~time)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~time)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F12">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>291.5582162745098</v>
+        <v>104.7037256315789</v>
       </c>
       <c r="H12">
-        <v>4.802447440153912</v>
+        <v>17.65712715009747</v>
       </c>
       <c r="I12">
-        <v>0.01914981962704228</v>
+        <v>4.878463237258471E-05</v>
       </c>
       <c r="J12">
-        <v>-545.75252</v>
+        <v>-54.726407</v>
       </c>
     </row>
     <row r="13">
@@ -879,7 +879,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -894,39 +894,39 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~sundur)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G13">
-        <v>292.01949</v>
+        <v>105.325859631579</v>
       </c>
       <c r="H13">
-        <v>5.263721165644085</v>
+        <v>18.27926115009747</v>
       </c>
       <c r="I13">
-        <v>0.01520548828227181</v>
+        <v>3.574278222194166E-05</v>
       </c>
       <c r="J13">
-        <v>-527.4755699999999</v>
+        <v>-54.104273</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -936,39 +936,39 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F14">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G14">
-        <v>293.0600264596274</v>
+        <v>105.691611631579</v>
       </c>
       <c r="H14">
-        <v>6.304257625271475</v>
+        <v>18.64501315009747</v>
       </c>
       <c r="I14">
-        <v>0.009037550760031529</v>
+        <v>2.976914197662823E-05</v>
       </c>
       <c r="J14">
-        <v>-524.0164</v>
+        <v>-53.738521</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -978,23 +978,23 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~wind)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F15">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15">
-        <v>293.5568964596274</v>
+        <v>105.7353426315789</v>
       </c>
       <c r="H15">
-        <v>6.801127625271477</v>
+        <v>18.68874415009746</v>
       </c>
       <c r="I15">
-        <v>0.007049475409602166</v>
+        <v>2.912528953250178E-05</v>
       </c>
       <c r="J15">
-        <v>-523.51953</v>
+        <v>-53.69479</v>
       </c>
     </row>
     <row r="16">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1020,23 +1020,23 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F16">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G16">
-        <v>294.4699325925926</v>
+        <v>107.2893546315789</v>
       </c>
       <c r="H16">
-        <v>7.714163758236737</v>
+        <v>20.24275615009746</v>
       </c>
       <c r="I16">
-        <v>0.00446574090881681</v>
+        <v>1.339124121898431E-05</v>
       </c>
       <c r="J16">
-        <v>-520.21772</v>
+        <v>-52.140778</v>
       </c>
     </row>
     <row r="17">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1062,23 +1062,23 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~wind)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~temp)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F17">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G17">
-        <v>295.0474225925926</v>
+        <v>108.7790596315789</v>
       </c>
       <c r="H17">
-        <v>8.291653758236748</v>
+        <v>21.73246115009746</v>
       </c>
       <c r="I17">
-        <v>0.003345747503713857</v>
+        <v>6.358219293604716E-06</v>
       </c>
       <c r="J17">
-        <v>-519.64023</v>
+        <v>-50.651073</v>
       </c>
     </row>
     <row r="18">
@@ -1089,12 +1089,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1104,23 +1104,23 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~1)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F18">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G18">
-        <v>299.4281385714286</v>
+        <v>109.4321176315789</v>
       </c>
       <c r="H18">
-        <v>12.6723697370727</v>
+        <v>22.38551915009747</v>
       </c>
       <c r="I18">
-        <v>0.0003743111588882351</v>
+        <v>4.586968520680744E-06</v>
       </c>
       <c r="J18">
-        <v>-535.23835</v>
+        <v>-49.998015</v>
       </c>
     </row>
     <row r="19">
@@ -1131,12 +1131,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1146,23 +1146,23 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~sundur + wind)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F19">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G19">
-        <v>299.7600076470588</v>
+        <v>111.0940512222222</v>
       </c>
       <c r="H19">
-        <v>13.00423881270297</v>
+        <v>24.04745274074074</v>
       </c>
       <c r="I19">
-        <v>0.0003170796135962569</v>
+        <v>1.99821155408167E-06</v>
       </c>
       <c r="J19">
-        <v>-496.82917</v>
+        <v>-54.137251</v>
       </c>
     </row>
     <row r="20">
@@ -1173,12 +1173,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1188,39 +1188,39 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp + sundur)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G20">
-        <v>299.8737618934912</v>
+        <v>111.1111282222222</v>
       </c>
       <c r="H20">
-        <v>13.1179930591353</v>
+        <v>24.06452974074074</v>
       </c>
       <c r="I20">
-        <v>0.0002995483277938715</v>
+        <v>1.981222458639957E-06</v>
       </c>
       <c r="J20">
-        <v>-498.88402</v>
+        <v>-54.120174</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1230,23 +1230,23 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F21">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21">
-        <v>299.9815425925926</v>
+        <v>111.4904902222222</v>
       </c>
       <c r="H21">
-        <v>13.22577375823676</v>
+        <v>24.44389174074075</v>
       </c>
       <c r="I21">
-        <v>0.000283832823891267</v>
+        <v>1.63891273832972E-06</v>
       </c>
       <c r="J21">
-        <v>-514.70611</v>
+        <v>-53.740812</v>
       </c>
     </row>
     <row r="22">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1272,34 +1272,34 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~temp + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F22">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G22">
-        <v>301.1674968421053</v>
+        <v>112.1771802222222</v>
       </c>
       <c r="H22">
-        <v>14.41172800774939</v>
+        <v>25.13058174074075</v>
       </c>
       <c r="I22">
-        <v>0.0001568685654218038</v>
+        <v>1.162633926627651E-06</v>
       </c>
       <c r="J22">
-        <v>-538.8223</v>
+        <v>-53.054122</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,23 +1314,23 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~sundur + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G23">
-        <v>301.6237471929825</v>
+        <v>112.9398762222222</v>
       </c>
       <c r="H23">
-        <v>14.8679783586266</v>
+        <v>25.89327774074073</v>
       </c>
       <c r="I23">
-        <v>0.0001248712387474658</v>
+        <v>7.94009429028247E-07</v>
       </c>
       <c r="J23">
-        <v>-492.82219</v>
+        <v>-52.291426</v>
       </c>
     </row>
     <row r="24">
@@ -1341,12 +1341,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1356,34 +1356,34 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~temp + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F24">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G24">
-        <v>301.6948462745098</v>
+        <v>114.4929812222222</v>
       </c>
       <c r="H24">
-        <v>14.93907744015388</v>
+        <v>27.44638274074075</v>
       </c>
       <c r="I24">
-        <v>0.0001205101010563231</v>
+        <v>3.652356773294304E-07</v>
       </c>
       <c r="J24">
-        <v>-535.6159</v>
+        <v>-50.738321</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1398,23 +1398,23 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F25">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G25">
-        <v>301.7950262745098</v>
+        <v>117.5645023529412</v>
       </c>
       <c r="H25">
-        <v>15.0392574401539</v>
+        <v>30.51790387145969</v>
       </c>
       <c r="I25">
-        <v>0.0001146224375907098</v>
+        <v>7.863227756384226E-08</v>
       </c>
       <c r="J25">
-        <v>-535.51572</v>
+        <v>-54.15046</v>
       </c>
     </row>
     <row r="26">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1440,23 +1440,23 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~1)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~temp + wind + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F26">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G26">
-        <v>301.9479188343558</v>
+        <v>118.4601333529412</v>
       </c>
       <c r="H26">
-        <v>15.19214999999997</v>
+        <v>31.41353487145969</v>
       </c>
       <c r="I26">
-        <v>0.0001061865333005682</v>
+        <v>5.02478003156237E-08</v>
       </c>
       <c r="J26">
-        <v>-510.38027</v>
+        <v>-53.254829</v>
       </c>
     </row>
     <row r="27">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1482,39 +1482,39 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur + wind)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~1)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F27">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G27">
-        <v>302.0838168421053</v>
+        <v>148.3504596153846</v>
       </c>
       <c r="H27">
-        <v>15.32804800774937</v>
+        <v>61.30386113390313</v>
       </c>
       <c r="I27">
-        <v>9.921094013344334E-05</v>
+        <v>1.623735087407893E-14</v>
       </c>
       <c r="J27">
-        <v>-537.90597</v>
+        <v>-59.274005</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1524,23 +1524,23 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~wind)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F28">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G28">
-        <v>302.6632876470588</v>
+        <v>159.5733643333333</v>
       </c>
       <c r="H28">
-        <v>15.90751881270296</v>
+        <v>72.52676585185185</v>
       </c>
       <c r="I28">
-        <v>7.425557724974242E-05</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>-493.92589</v>
+        <v>-60.769049</v>
       </c>
     </row>
     <row r="29">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1566,23 +1566,23 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~temp)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F29">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G29">
-        <v>304.4148615231788</v>
+        <v>160.8222343333333</v>
       </c>
       <c r="H29">
-        <v>17.65909268882291</v>
+        <v>73.77563585185186</v>
       </c>
       <c r="I29">
-        <v>3.092998034645175E-05</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>-538.2894700000001</v>
+        <v>-59.520179</v>
       </c>
     </row>
     <row r="30">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1608,29 +1608,29 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~sundur)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F30">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G30">
-        <v>305.2379268421053</v>
+        <v>160.8692983333333</v>
       </c>
       <c r="H30">
-        <v>18.48215800774938</v>
+        <v>73.82269985185187</v>
       </c>
       <c r="I30">
-        <v>2.049525286593902E-05</v>
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>-534.7518700000001</v>
+        <v>-59.473115</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1650,34 +1650,34 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~time)pent(~time)N(~1)</t>
+          <t>Phi(~time)p(~time)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F31">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G31">
-        <v>306.4286462745098</v>
+        <v>160.9105593333333</v>
       </c>
       <c r="H31">
-        <v>19.67287744015391</v>
+        <v>73.86396085185186</v>
       </c>
       <c r="I31">
-        <v>1.130034860916514E-05</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>-530.8821</v>
+        <v>-59.431854</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1692,39 +1692,39 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~wind)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~time)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F32">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G32">
-        <v>306.8022562745098</v>
+        <v>161.2669543333333</v>
       </c>
       <c r="H32">
-        <v>20.0464874401539</v>
+        <v>74.22035585185185</v>
       </c>
       <c r="I32">
-        <v>9.374831286717117E-06</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>-530.5084900000001</v>
+        <v>-59.075459</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1734,39 +1734,39 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~1)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~temp + wind)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F33">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G33">
-        <v>308.6874181395349</v>
+        <v>172.5183543636364</v>
       </c>
       <c r="H33">
-        <v>21.93164930517901</v>
+        <v>85.47175588215489</v>
       </c>
       <c r="I33">
-        <v>3.652630683147479E-06</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>-483.6402</v>
+        <v>-62.854361</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1776,39 +1776,39 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~sundur + wind)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F34">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G34">
-        <v>309.3177771929825</v>
+        <v>174.5819133636364</v>
       </c>
       <c r="H34">
-        <v>22.5620083586266</v>
+        <v>87.53531488215489</v>
       </c>
       <c r="I34">
-        <v>2.665170722055138E-06</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>-485.12816</v>
+        <v>-60.790803</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1818,39 +1818,39 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~wind)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~temp + sundur)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G35">
-        <v>310.0744971929824</v>
+        <v>175.3834563636364</v>
       </c>
       <c r="H35">
-        <v>23.31872835862657</v>
+        <v>88.33685788215487</v>
       </c>
       <c r="I35">
-        <v>1.825598934304528E-06</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>-484.37144</v>
+        <v>-59.98926</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~time</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1860,23 +1860,23 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur + wind)pent(~1)N(~1)</t>
+          <t>Phi(~time)p(~temp + wind + sundur)pent(~time)N(~1)</t>
         </is>
       </c>
       <c r="F36">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="G36">
-        <v>310.5573376470588</v>
+        <v>190.55124</v>
       </c>
       <c r="H36">
-        <v>23.80156881270295</v>
+        <v>103.5046415185185</v>
       </c>
       <c r="I36">
-        <v>1.434028891317156E-06</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>-486.03183</v>
+        <v>-62.85784</v>
       </c>
     </row>
     <row r="37">
@@ -1906,19 +1906,19 @@
         </is>
       </c>
       <c r="F37">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G37">
-        <v>314.1371666666667</v>
+        <v>386.937527</v>
       </c>
       <c r="H37">
-        <v>27.38139783231082</v>
+        <v>299.8909285185185</v>
       </c>
       <c r="I37">
-        <v>2.394461764273403E-07</v>
+        <v>0</v>
       </c>
       <c r="J37">
-        <v>-548.62456</v>
+        <v>-64.87155300000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes revision 3
</commit_message>
<xml_diff>
--- a/data/population_models/models_output_kriegberg.xlsx
+++ b/data/population_models/models_output_kriegberg.xlsx
@@ -412,17 +412,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -432,34 +432,34 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~Time)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G2">
-        <v>81.6623863076923</v>
+        <v>271.7338443113773</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.1836889152358518</v>
+        <v>0.3839741921345565</v>
       </c>
       <c r="J2">
-        <v>-49.654386</v>
+        <v>-531.43906</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -474,39 +474,39 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~1)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <v>82.89809330769231</v>
+        <v>273.2132712048193</v>
       </c>
       <c r="H3">
-        <v>1.235707000000005</v>
+        <v>1.479426893441996</v>
       </c>
       <c r="I3">
-        <v>0.09902676317819152</v>
+        <v>0.1832519341880248</v>
       </c>
       <c r="J3">
-        <v>-48.418678</v>
+        <v>-532.20709</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -516,34 +516,34 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~Time + I(Time^2))pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~Time)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>83.177047</v>
+        <v>274.4731243113773</v>
       </c>
       <c r="H4">
-        <v>1.5146606923077</v>
+        <v>2.739280000000008</v>
       </c>
       <c r="I4">
-        <v>0.08613478205130892</v>
+        <v>0.09760564621860626</v>
       </c>
       <c r="J4">
-        <v>-51.192033</v>
+        <v>-528.69978</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -558,39 +558,39 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~1)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>84.3708523076923</v>
+        <v>274.6359228571428</v>
       </c>
       <c r="H5">
-        <v>2.708466000000001</v>
+        <v>2.902078545765562</v>
       </c>
       <c r="I5">
-        <v>0.047418414685642</v>
+        <v>0.0899753792902651</v>
       </c>
       <c r="J5">
-        <v>-46.94592</v>
+        <v>-526.31628</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -600,39 +600,39 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~1)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>84.381186</v>
+        <v>275.3672800000001</v>
       </c>
       <c r="H6">
-        <v>2.718799692307698</v>
+        <v>3.633435688622797</v>
       </c>
       <c r="I6">
-        <v>0.04717404289148591</v>
+        <v>0.06241823735850541</v>
       </c>
       <c r="J6">
-        <v>-49.987894</v>
+        <v>-532.32778</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -642,39 +642,39 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~Time)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>84.47165</v>
+        <v>275.4928543113772</v>
       </c>
       <c r="H7">
-        <v>2.809263692307695</v>
+        <v>3.759009999999989</v>
       </c>
       <c r="I7">
-        <v>0.04508780462797671</v>
+        <v>0.05861967214297935</v>
       </c>
       <c r="J7">
-        <v>-49.89743</v>
+        <v>-527.6800500000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -684,34 +684,34 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~Time)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>84.714651</v>
+        <v>275.8077012048192</v>
       </c>
       <c r="H8">
-        <v>3.052264692307702</v>
+        <v>4.073856893441985</v>
       </c>
       <c r="I8">
-        <v>0.03992933642900449</v>
+        <v>0.0500812604710393</v>
       </c>
       <c r="J8">
-        <v>-49.654429</v>
+        <v>-529.61265</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -726,39 +726,39 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~1)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G9">
-        <v>84.980071</v>
+        <v>278.0846112048193</v>
       </c>
       <c r="H9">
-        <v>3.317684692307694</v>
+        <v>6.350766893442028</v>
       </c>
       <c r="I9">
-        <v>0.03496687911939016</v>
+        <v>0.01604170503333236</v>
       </c>
       <c r="J9">
-        <v>-49.389009</v>
+        <v>-527.33574</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -768,39 +768,39 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~Time + I(Time^2))pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F10">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G10">
-        <v>85.59003166666668</v>
+        <v>278.8064443113772</v>
       </c>
       <c r="H10">
-        <v>3.927645358974374</v>
+        <v>7.072599999999966</v>
       </c>
       <c r="I10">
-        <v>0.02577541083985738</v>
+        <v>0.01118166454214482</v>
       </c>
       <c r="J10">
-        <v>-52.085715</v>
+        <v>-524.36646</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -810,39 +810,39 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>85.618628</v>
+        <v>278.8148143113772</v>
       </c>
       <c r="H11">
-        <v>3.9562416923077</v>
+        <v>7.080969999999979</v>
       </c>
       <c r="I11">
-        <v>0.02540949193842995</v>
+        <v>0.01113496705867586</v>
       </c>
       <c r="J11">
-        <v>-48.750452</v>
+        <v>-524.3580899999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -852,39 +852,39 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G12">
-        <v>85.847545</v>
+        <v>278.9150528571428</v>
       </c>
       <c r="H12">
-        <v>4.185158692307695</v>
+        <v>7.181208545765571</v>
       </c>
       <c r="I12">
-        <v>0.02266142868960756</v>
+        <v>0.01059064505495791</v>
       </c>
       <c r="J12">
-        <v>-48.521535</v>
+        <v>-522.03715</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -894,39 +894,39 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~1)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G13">
-        <v>85.923945</v>
+        <v>279.2729628571428</v>
       </c>
       <c r="H13">
-        <v>4.261558692307702</v>
+        <v>7.539118545765575</v>
       </c>
       <c r="I13">
-        <v>0.02181208780473643</v>
+        <v>0.008855299288372455</v>
       </c>
       <c r="J13">
-        <v>-48.445135</v>
+        <v>-521.67924</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -936,39 +936,39 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~1)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>86.02094766666667</v>
+        <v>281.1350443113773</v>
       </c>
       <c r="H14">
-        <v>4.35856135897437</v>
+        <v>9.401200000000017</v>
       </c>
       <c r="I14">
-        <v>0.02077941782685654</v>
+        <v>0.00349025689485473</v>
       </c>
       <c r="J14">
-        <v>-51.654799</v>
+        <v>-522.03785</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -978,39 +978,39 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~Time + I(Time^2))pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~temp)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>86.42020466666668</v>
+        <v>282.4844928571428</v>
       </c>
       <c r="H15">
-        <v>4.757818358974376</v>
+        <v>10.75064854576556</v>
       </c>
       <c r="I15">
-        <v>0.01701906981606627</v>
+        <v>0.001777576766138115</v>
       </c>
       <c r="J15">
-        <v>-51.255542</v>
+        <v>-518.46771</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1020,23 +1020,23 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>86.541254</v>
+        <v>282.6734112048193</v>
       </c>
       <c r="H16">
-        <v>4.878867692307693</v>
+        <v>10.93956689344202</v>
       </c>
       <c r="I16">
-        <v>0.01601954921859827</v>
+        <v>0.001617354671294887</v>
       </c>
       <c r="J16">
-        <v>-47.827826</v>
+        <v>-522.74695</v>
       </c>
     </row>
     <row r="17">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1062,23 +1062,23 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~Time)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F17">
         <v>7</v>
       </c>
       <c r="G17">
-        <v>86.84018066666667</v>
+        <v>284.0314018934911</v>
       </c>
       <c r="H17">
-        <v>5.177794358974367</v>
+        <v>12.29755758211388</v>
       </c>
       <c r="I17">
-        <v>0.01379555541964187</v>
+        <v>0.0008202029669258829</v>
       </c>
       <c r="J17">
-        <v>-50.835566</v>
+        <v>-514.72637</v>
       </c>
     </row>
     <row r="18">
@@ -1089,12 +1089,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1104,39 +1104,39 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F18">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G18">
-        <v>86.850617</v>
+        <v>284.4148943113772</v>
       </c>
       <c r="H18">
-        <v>5.188230692307698</v>
+        <v>12.68104999999997</v>
       </c>
       <c r="I18">
-        <v>0.0137237554073401</v>
+        <v>0.0006770909599877416</v>
       </c>
       <c r="J18">
-        <v>-47.518462</v>
+        <v>-518.75801</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1146,39 +1146,39 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G19">
-        <v>86.97204166666667</v>
+        <v>284.4690343113772</v>
       </c>
       <c r="H19">
-        <v>5.309655358974368</v>
+        <v>12.73518999999999</v>
       </c>
       <c r="I19">
-        <v>0.01291534280350566</v>
+        <v>0.0006590079652663915</v>
       </c>
       <c r="J19">
-        <v>-50.703705</v>
+        <v>-518.7038700000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1188,39 +1188,39 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~1)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G20">
-        <v>87.04659848148148</v>
+        <v>284.7085043113772</v>
       </c>
       <c r="H20">
-        <v>5.38421217378918</v>
+        <v>12.97465999999997</v>
       </c>
       <c r="I20">
-        <v>0.01244274300550185</v>
+        <v>0.0005846425421013672</v>
       </c>
       <c r="J20">
-        <v>-41.443963</v>
+        <v>-518.46439</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1230,39 +1230,39 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G21">
-        <v>87.1192323076923</v>
+        <v>284.7444028571429</v>
       </c>
       <c r="H21">
-        <v>5.456845999999999</v>
+        <v>13.0105585457656</v>
       </c>
       <c r="I21">
-        <v>0.0119989680317264</v>
+        <v>0.0005742422516260308</v>
       </c>
       <c r="J21">
-        <v>-44.19754</v>
+        <v>-516.2078</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1272,39 +1272,39 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~1)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G22">
-        <v>87.22297399999999</v>
+        <v>284.7557928571428</v>
       </c>
       <c r="H22">
-        <v>5.560587692307692</v>
+        <v>13.02194854576555</v>
       </c>
       <c r="I22">
-        <v>0.01139243800701563</v>
+        <v>0.0005709812365571542</v>
       </c>
       <c r="J22">
-        <v>-47.146106</v>
+        <v>-516.19641</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1314,39 +1314,39 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G23">
-        <v>87.422478</v>
+        <v>284.8073328571429</v>
       </c>
       <c r="H23">
-        <v>5.760091692307697</v>
+        <v>13.0734885457656</v>
       </c>
       <c r="I23">
-        <v>0.01031086096786938</v>
+        <v>0.0005564550242242812</v>
       </c>
       <c r="J23">
-        <v>-46.946602</v>
+        <v>-516.14487</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1356,39 +1356,39 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~Time + I(Time^2))pent(~Time)N(~1)</t>
+          <t>Phi(~1)p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F24">
         <v>8</v>
       </c>
       <c r="G24">
-        <v>87.47496956521739</v>
+        <v>284.8321828571428</v>
       </c>
       <c r="H24">
-        <v>5.812583257525091</v>
+        <v>13.09833854576556</v>
       </c>
       <c r="I24">
-        <v>0.01004376475897656</v>
+        <v>0.0005495838461399913</v>
       </c>
       <c r="J24">
-        <v>-53.79498</v>
+        <v>-516.12002</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1398,23 +1398,23 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~Time)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F25">
         <v>7</v>
       </c>
       <c r="G25">
-        <v>87.59111666666666</v>
+        <v>284.8413018934912</v>
       </c>
       <c r="H25">
-        <v>5.928730358974363</v>
+        <v>13.10745758211391</v>
       </c>
       <c r="I25">
-        <v>0.009477101013593996</v>
+        <v>0.0005470837126386654</v>
       </c>
       <c r="J25">
-        <v>-50.08463</v>
+        <v>-513.91648</v>
       </c>
     </row>
     <row r="26">
@@ -1425,12 +1425,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1440,29 +1440,29 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp)pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F26">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G26">
-        <v>87.63813866666668</v>
+        <v>285.0953812048193</v>
       </c>
       <c r="H26">
-        <v>5.975752358974376</v>
+        <v>13.36153689344201</v>
       </c>
       <c r="I26">
-        <v>0.009256883799104445</v>
+        <v>0.0004818159403404257</v>
       </c>
       <c r="J26">
-        <v>-50.037608</v>
+        <v>-520.32498</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1482,39 +1482,39 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F27">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G27">
-        <v>87.64102866666667</v>
+        <v>285.1121028571428</v>
       </c>
       <c r="H27">
-        <v>5.978642358974369</v>
+        <v>13.37825854576556</v>
       </c>
       <c r="I27">
-        <v>0.009243517261663874</v>
+        <v>0.0004778043544758912</v>
       </c>
       <c r="J27">
-        <v>-50.034718</v>
+        <v>-515.8401</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1524,39 +1524,39 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~1)pent(~Time)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G28">
-        <v>87.66043966666668</v>
+        <v>285.2874243113773</v>
       </c>
       <c r="H28">
-        <v>5.998053358974374</v>
+        <v>13.55358000000001</v>
       </c>
       <c r="I28">
-        <v>0.00915423825439806</v>
+        <v>0.0004377030101308192</v>
       </c>
       <c r="J28">
-        <v>-50.015307</v>
+        <v>-517.88548</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G29">
-        <v>87.66665166666667</v>
+        <v>285.4975143113772</v>
       </c>
       <c r="H29">
-        <v>6.004265358974365</v>
+        <v>13.76366999999999</v>
       </c>
       <c r="I29">
-        <v>0.009125849301247093</v>
+        <v>0.0003940570206656865</v>
       </c>
       <c r="J29">
-        <v>-50.009095</v>
+        <v>-517.67539</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1608,39 +1608,39 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~Time)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>87.75777066666667</v>
+        <v>285.5656143113773</v>
       </c>
       <c r="H30">
-        <v>6.095384358974371</v>
+        <v>13.83177000000001</v>
       </c>
       <c r="I30">
-        <v>0.008719409077184301</v>
+        <v>0.0003808652436395312</v>
       </c>
       <c r="J30">
-        <v>-49.917976</v>
+        <v>-517.60729</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1650,39 +1650,39 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F31">
         <v>7</v>
       </c>
       <c r="G31">
-        <v>88.20757366666668</v>
+        <v>285.6255418934912</v>
       </c>
       <c r="H31">
-        <v>6.545187358974374</v>
+        <v>13.89169758211392</v>
       </c>
       <c r="I31">
-        <v>0.006963275414979152</v>
+        <v>0.0003696223579664537</v>
       </c>
       <c r="J31">
-        <v>-49.468173</v>
+        <v>-513.13224</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1692,39 +1692,39 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~sundur + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G32">
-        <v>88.26712966666668</v>
+        <v>286.9403228571429</v>
       </c>
       <c r="H32">
-        <v>6.604743358974375</v>
+        <v>15.20647854576561</v>
       </c>
       <c r="I32">
-        <v>0.006758979852319409</v>
+        <v>0.0001915389818435082</v>
       </c>
       <c r="J32">
-        <v>-49.408617</v>
+        <v>-514.01188</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1734,39 +1734,39 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G33">
-        <v>88.73760166666668</v>
+        <v>287.0640228571428</v>
       </c>
       <c r="H33">
-        <v>7.075215358974376</v>
+        <v>15.33017854576559</v>
       </c>
       <c r="I33">
-        <v>0.005342191538487522</v>
+        <v>0.0001800512168451556</v>
       </c>
       <c r="J33">
-        <v>-48.938145</v>
+        <v>-513.88818</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1776,34 +1776,34 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F34">
         <v>7</v>
       </c>
       <c r="G34">
-        <v>88.80669966666667</v>
+        <v>287.2141718934911</v>
       </c>
       <c r="H34">
-        <v>7.144313358974372</v>
+        <v>15.48032758211389</v>
       </c>
       <c r="I34">
-        <v>0.005160776069481624</v>
+        <v>0.0001670288964814634</v>
       </c>
       <c r="J34">
-        <v>-48.869046</v>
+        <v>-511.5436</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1818,39 +1818,39 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F35">
         <v>8</v>
       </c>
       <c r="G35">
-        <v>88.99667456521739</v>
+        <v>287.5842128571429</v>
       </c>
       <c r="H35">
-        <v>7.334288257525088</v>
+        <v>15.8503685457656</v>
       </c>
       <c r="I35">
-        <v>0.00469312898023784</v>
+        <v>0.000138815588167017</v>
       </c>
       <c r="J35">
-        <v>-52.273275</v>
+        <v>-513.36799</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1860,34 +1860,34 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G36">
-        <v>89.0723425652174</v>
+        <v>288.5505618934911</v>
       </c>
       <c r="H36">
-        <v>7.409956257525096</v>
+        <v>16.81671758211388</v>
       </c>
       <c r="I36">
-        <v>0.004518886075377215</v>
+        <v>8.562453194840419E-05</v>
       </c>
       <c r="J36">
-        <v>-52.197607</v>
+        <v>-510.20722</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1902,39 +1902,39 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur + wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F37">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G37">
-        <v>89.10792366666666</v>
+        <v>289.2980643113772</v>
       </c>
       <c r="H37">
-        <v>7.445537358974363</v>
+        <v>17.56421999999998</v>
       </c>
       <c r="I37">
-        <v>0.004439203503494138</v>
+        <v>5.892235859913179E-05</v>
       </c>
       <c r="J37">
-        <v>-48.567823</v>
+        <v>-513.87483</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1944,29 +1944,29 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + wind)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F38">
         <v>7</v>
       </c>
       <c r="G38">
-        <v>89.30220366666667</v>
+        <v>289.3234318934911</v>
       </c>
       <c r="H38">
-        <v>7.639817358974369</v>
+        <v>17.58958758211389</v>
       </c>
       <c r="I38">
-        <v>0.004028261805912323</v>
+        <v>5.817971941042734E-05</v>
       </c>
       <c r="J38">
-        <v>-48.373543</v>
+        <v>-509.43435</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1986,29 +1986,29 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G39">
-        <v>89.49217956521738</v>
+        <v>290.3218518934912</v>
       </c>
       <c r="H39">
-        <v>7.829793257525083</v>
+        <v>18.5880075821139</v>
       </c>
       <c r="I39">
-        <v>0.003663236403636003</v>
+        <v>3.531567195939614E-05</v>
       </c>
       <c r="J39">
-        <v>-51.77777</v>
+        <v>-508.43592</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2028,39 +2028,39 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~Time)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~Time)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F40">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40">
-        <v>89.55540156521739</v>
+        <v>290.3721318934911</v>
       </c>
       <c r="H40">
-        <v>7.893015257525093</v>
+        <v>18.63828758211389</v>
       </c>
       <c r="I40">
-        <v>0.003549248957975098</v>
+        <v>3.443890312798542E-05</v>
       </c>
       <c r="J40">
-        <v>-51.714548</v>
+        <v>-508.38565</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2070,23 +2070,23 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~1)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F41">
         <v>8</v>
       </c>
       <c r="G41">
-        <v>89.60539756521739</v>
+        <v>290.4219828571428</v>
       </c>
       <c r="H41">
-        <v>7.943011257525086</v>
+        <v>18.68813854576558</v>
       </c>
       <c r="I41">
-        <v>0.003461624612211657</v>
+        <v>3.359110663477926E-05</v>
       </c>
       <c r="J41">
-        <v>-51.664552</v>
+        <v>-510.53022</v>
       </c>
     </row>
     <row r="42">
@@ -2097,12 +2097,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2112,39 +2112,39 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~Time)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F42">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G42">
-        <v>89.60951856521739</v>
+        <v>290.4754276470588</v>
       </c>
       <c r="H42">
-        <v>7.947132257525084</v>
+        <v>18.74158333568158</v>
       </c>
       <c r="I42">
-        <v>0.003454499278094651</v>
+        <v>3.27053591707159E-05</v>
       </c>
       <c r="J42">
-        <v>-51.660431</v>
+        <v>-506.11375</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2154,23 +2154,23 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G43">
-        <v>89.78593166666667</v>
+        <v>290.4858476470588</v>
       </c>
       <c r="H43">
-        <v>8.123545358974368</v>
+        <v>18.75200333568159</v>
       </c>
       <c r="I43">
-        <v>0.003162841932781782</v>
+        <v>3.253540735833978E-05</v>
       </c>
       <c r="J43">
-        <v>-47.889815</v>
+        <v>-506.10333</v>
       </c>
     </row>
     <row r="44">
@@ -2181,12 +2181,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2196,39 +2196,39 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F44">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G44">
-        <v>89.83976266666667</v>
+        <v>291.4996143113772</v>
       </c>
       <c r="H44">
-        <v>8.177376358974371</v>
+        <v>19.76576999999997</v>
       </c>
       <c r="I44">
-        <v>0.003078847902093868</v>
+        <v>1.959835474885785E-05</v>
       </c>
       <c r="J44">
-        <v>-47.835984</v>
+        <v>-511.67329</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2238,34 +2238,34 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~Time)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F45">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G45">
-        <v>89.86769930769231</v>
+        <v>291.5251018934911</v>
       </c>
       <c r="H45">
-        <v>8.205313000000004</v>
+        <v>19.79125758211387</v>
       </c>
       <c r="I45">
-        <v>0.003036140537265362</v>
+        <v>1.935018209975275E-05</v>
       </c>
       <c r="J45">
-        <v>-41.449073</v>
+        <v>-507.23267</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2280,39 +2280,39 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F46">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G46">
-        <v>89.87052730769231</v>
+        <v>291.6295928571428</v>
       </c>
       <c r="H46">
-        <v>8.208141000000012</v>
+        <v>19.89574854576557</v>
       </c>
       <c r="I46">
-        <v>0.003031850468339182</v>
+        <v>1.836517757523836E-05</v>
       </c>
       <c r="J46">
-        <v>-41.446245</v>
+        <v>-509.32261</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2322,23 +2322,23 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~Time)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F47">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G47">
-        <v>89.94076099999999</v>
+        <v>291.6332528571428</v>
       </c>
       <c r="H47">
-        <v>8.278374692307693</v>
+        <v>19.8994085457656</v>
       </c>
       <c r="I47">
-        <v>0.002927229178056945</v>
+        <v>1.833160003309716E-05</v>
       </c>
       <c r="J47">
-        <v>-44.428319</v>
+        <v>-509.31895</v>
       </c>
     </row>
     <row r="48">
@@ -2349,12 +2349,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2364,39 +2364,39 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~sundur + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F48">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G48">
-        <v>89.9858425652174</v>
+        <v>292.1202018934911</v>
       </c>
       <c r="H48">
-        <v>8.323456257525095</v>
+        <v>20.38635758211387</v>
       </c>
       <c r="I48">
-        <v>0.002861985228789829</v>
+        <v>1.437013120129287E-05</v>
       </c>
       <c r="J48">
-        <v>-51.284107</v>
+        <v>-506.63757</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2406,39 +2406,39 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~1)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G49">
-        <v>90.01003366666667</v>
+        <v>292.1783876470589</v>
       </c>
       <c r="H49">
-        <v>8.34764735897437</v>
+        <v>20.4445433356816</v>
       </c>
       <c r="I49">
-        <v>0.002827576457308231</v>
+        <v>1.395808560317769E-05</v>
       </c>
       <c r="J49">
-        <v>-47.665713</v>
+        <v>-504.41079</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2448,23 +2448,23 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G50">
-        <v>90.13548400000001</v>
+        <v>292.4531218934911</v>
       </c>
       <c r="H50">
-        <v>8.473097692307704</v>
+        <v>20.71927758211388</v>
       </c>
       <c r="I50">
-        <v>0.002655664225711535</v>
+        <v>1.216656761034171E-05</v>
       </c>
       <c r="J50">
-        <v>-44.233596</v>
+        <v>-506.30466</v>
       </c>
     </row>
     <row r="51">
@@ -2475,7 +2475,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2490,23 +2490,23 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~sundur + wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F51">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G51">
-        <v>90.14225466666667</v>
+        <v>292.5205676470588</v>
       </c>
       <c r="H51">
-        <v>8.479868358974372</v>
+        <v>20.78672333568159</v>
       </c>
       <c r="I51">
-        <v>0.002646689117524137</v>
+        <v>1.176311694255499E-05</v>
       </c>
       <c r="J51">
-        <v>-47.533492</v>
+        <v>-504.06861</v>
       </c>
     </row>
     <row r="52">
@@ -2517,12 +2517,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2532,39 +2532,39 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~sundur + wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~Time + I(Time^2))pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F52">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G52">
-        <v>90.36301656521739</v>
+        <v>292.6249218934911</v>
       </c>
       <c r="H52">
-        <v>8.700630257525091</v>
+        <v>20.89107758211389</v>
       </c>
       <c r="I52">
-        <v>0.002370091400395992</v>
+        <v>1.11650887060464E-05</v>
       </c>
       <c r="J52">
-        <v>-50.906933</v>
+        <v>-506.13286</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2574,23 +2574,23 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~Time + I(Time^2))pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F53">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G53">
-        <v>90.52933566666667</v>
+        <v>292.7317228571428</v>
       </c>
       <c r="H53">
-        <v>8.866949358974367</v>
+        <v>20.99787854576556</v>
       </c>
       <c r="I53">
-        <v>0.002180968336531183</v>
+        <v>1.058450721471629E-05</v>
       </c>
       <c r="J53">
-        <v>-47.146411</v>
+        <v>-508.22048</v>
       </c>
     </row>
     <row r="54">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2616,34 +2616,34 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~1)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F54">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54">
-        <v>90.5320985652174</v>
+        <v>293.0105718934911</v>
       </c>
       <c r="H54">
-        <v>8.869712257525094</v>
+        <v>21.27672758211389</v>
       </c>
       <c r="I54">
-        <v>0.002177957519527395</v>
+        <v>9.207025466281654E-06</v>
       </c>
       <c r="J54">
-        <v>-50.737851</v>
+        <v>-505.74721</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2658,29 +2658,29 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F55">
         <v>8</v>
       </c>
       <c r="G55">
-        <v>90.56624256521739</v>
+        <v>293.5443728571428</v>
       </c>
       <c r="H55">
-        <v>8.903856257525092</v>
+        <v>21.81052854576558</v>
       </c>
       <c r="I55">
-        <v>0.002141091016623436</v>
+        <v>7.050273063219025E-06</v>
       </c>
       <c r="J55">
-        <v>-50.703707</v>
+        <v>-507.40783</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2700,39 +2700,39 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~Time)pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~Time)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F56">
         <v>8</v>
       </c>
       <c r="G56">
-        <v>90.98564856521739</v>
+        <v>293.6260828571428</v>
       </c>
       <c r="H56">
-        <v>9.323262257525087</v>
+        <v>21.89223854576557</v>
       </c>
       <c r="I56">
-        <v>0.001736050177605957</v>
+        <v>6.768038754637819E-06</v>
       </c>
       <c r="J56">
-        <v>-50.284301</v>
+        <v>-507.32612</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2742,39 +2742,39 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F57">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G57">
-        <v>91.11562456521739</v>
+        <v>293.6904512048193</v>
       </c>
       <c r="H57">
-        <v>9.453238257525086</v>
+        <v>21.95660689344203</v>
       </c>
       <c r="I57">
-        <v>0.00162681565789587</v>
+        <v>6.553682953532421E-06</v>
       </c>
       <c r="J57">
-        <v>-50.154325</v>
+        <v>-511.72991</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2784,34 +2784,34 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F58">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G58">
-        <v>91.14257556521738</v>
+        <v>293.7127476470588</v>
       </c>
       <c r="H58">
-        <v>9.480189257525083</v>
+        <v>21.97890333568159</v>
       </c>
       <c r="I58">
-        <v>0.001605040548252116</v>
+        <v>6.481026792781613E-06</v>
       </c>
       <c r="J58">
-        <v>-50.127374</v>
+        <v>-502.87643</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2826,23 +2826,23 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F59">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G59">
-        <v>91.21510756521739</v>
+        <v>293.9077118934911</v>
       </c>
       <c r="H59">
-        <v>9.552721257525093</v>
+        <v>22.17386758211387</v>
       </c>
       <c r="I59">
-        <v>0.001547874996003712</v>
+        <v>5.879059677157837E-06</v>
       </c>
       <c r="J59">
-        <v>-50.054842</v>
+        <v>-504.85006</v>
       </c>
     </row>
     <row r="60">
@@ -2875,32 +2875,32 @@
         <v>8</v>
       </c>
       <c r="G60">
-        <v>91.21925256521739</v>
+        <v>294.0425428571428</v>
       </c>
       <c r="H60">
-        <v>9.556866257525087</v>
+        <v>22.30869854576559</v>
       </c>
       <c r="I60">
-        <v>0.001544670347039054</v>
+        <v>5.495784525440368E-06</v>
       </c>
       <c r="J60">
-        <v>-50.050697</v>
+        <v>-506.90966</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2910,23 +2910,23 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F61">
         <v>8</v>
       </c>
       <c r="G61">
-        <v>91.22915756521739</v>
+        <v>294.0865128571428</v>
       </c>
       <c r="H61">
-        <v>9.56677125752509</v>
+        <v>22.3526685457656</v>
       </c>
       <c r="I61">
-        <v>0.001537039279174563</v>
+        <v>5.376278189525598E-06</v>
       </c>
       <c r="J61">
-        <v>-50.040792</v>
+        <v>-506.86569</v>
       </c>
     </row>
     <row r="62">
@@ -2937,12 +2937,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2952,39 +2952,39 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F62">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G62">
-        <v>91.32130218181818</v>
+        <v>294.1669518934912</v>
       </c>
       <c r="H62">
-        <v>9.658915874125881</v>
+        <v>22.43310758211391</v>
       </c>
       <c r="I62">
-        <v>0.001467830868954312</v>
+        <v>5.164337516059679E-06</v>
       </c>
       <c r="J62">
-        <v>-53.869596</v>
+        <v>-504.59083</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2994,34 +2994,34 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~1)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F63">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G63">
-        <v>91.34339218181819</v>
+        <v>294.1767918934912</v>
       </c>
       <c r="H63">
-        <v>9.681005874125887</v>
+        <v>22.4429475821139</v>
       </c>
       <c r="I63">
-        <v>0.001451707880118558</v>
+        <v>5.138991378108242E-06</v>
       </c>
       <c r="J63">
-        <v>-53.847506</v>
+        <v>-504.58099</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3036,23 +3036,23 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F64">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G64">
-        <v>91.7918755652174</v>
+        <v>294.8890043113772</v>
       </c>
       <c r="H64">
-        <v>10.12948925752509</v>
+        <v>23.15515999999997</v>
       </c>
       <c r="I64">
-        <v>0.001160091660850788</v>
+        <v>3.599340453543057E-06</v>
       </c>
       <c r="J64">
-        <v>-49.478074</v>
+        <v>-508.28389</v>
       </c>
     </row>
     <row r="65">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3078,34 +3078,34 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind + sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~1)p(~1)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F65">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G65">
-        <v>92.1385295652174</v>
+        <v>294.9622271929825</v>
       </c>
       <c r="H65">
-        <v>10.4761432575251</v>
+        <v>23.22838288160523</v>
       </c>
       <c r="I65">
-        <v>0.0009754776992424042</v>
+        <v>3.469946515799674E-06</v>
       </c>
       <c r="J65">
-        <v>-49.13142</v>
+        <v>-499.48371</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3120,34 +3120,34 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + wind + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~1)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F66">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G66">
-        <v>92.74816756521739</v>
+        <v>294.9773376470588</v>
       </c>
       <c r="H66">
-        <v>11.08578125752508</v>
+        <v>23.24349333568159</v>
       </c>
       <c r="I66">
-        <v>0.0007191775726702218</v>
+        <v>3.44382906792169E-06</v>
       </c>
       <c r="J66">
-        <v>-48.521782</v>
+        <v>-501.61184</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3162,23 +3162,23 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~sundur + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F67">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G67">
-        <v>92.8962525652174</v>
+        <v>295.0537018934912</v>
       </c>
       <c r="H67">
-        <v>11.23386625752509</v>
+        <v>23.31985758211391</v>
       </c>
       <c r="I67">
-        <v>0.000667851470293668</v>
+        <v>3.314815050149916E-06</v>
       </c>
       <c r="J67">
-        <v>-48.373697</v>
+        <v>-503.70407</v>
       </c>
     </row>
     <row r="68">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3204,34 +3204,34 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur + wind)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~Time + I(Time^2))pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F68">
         <v>6</v>
       </c>
       <c r="G68">
-        <v>92.917738</v>
+        <v>295.0603476470588</v>
       </c>
       <c r="H68">
-        <v>11.2553516923077</v>
+        <v>23.32650333568159</v>
       </c>
       <c r="I68">
-        <v>0.0006607153300869938</v>
+        <v>3.303818608205974E-06</v>
       </c>
       <c r="J68">
-        <v>-41.451341</v>
+        <v>-501.52883</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3246,39 +3246,39 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~1)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F69">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G69">
-        <v>92.91841718181819</v>
+        <v>295.1019776470588</v>
       </c>
       <c r="H69">
-        <v>11.25603087412588</v>
+        <v>23.36813333568159</v>
       </c>
       <c r="I69">
-        <v>0.0006604909952605878</v>
+        <v>3.235760396957673E-06</v>
       </c>
       <c r="J69">
-        <v>-52.27248</v>
+        <v>-501.48719</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3288,39 +3288,39 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~temp)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F70">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G70">
-        <v>92.93703718181818</v>
+        <v>295.1930376470588</v>
       </c>
       <c r="H70">
-        <v>11.27465087412588</v>
+        <v>23.45919333568156</v>
       </c>
       <c r="I70">
-        <v>0.0006543703598618302</v>
+        <v>3.091739734935766E-06</v>
       </c>
       <c r="J70">
-        <v>-52.253861</v>
+        <v>-501.39614</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3330,23 +3330,23 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~Time + I(Time^2))pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F71">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G71">
-        <v>92.98202118181818</v>
+        <v>295.9193618934912</v>
       </c>
       <c r="H71">
-        <v>11.31963487412588</v>
+        <v>24.1855175821139</v>
       </c>
       <c r="I71">
-        <v>0.0006398165474494589</v>
+        <v>2.150223586108443E-06</v>
       </c>
       <c r="J71">
-        <v>-52.208877</v>
+        <v>-502.83842</v>
       </c>
     </row>
     <row r="72">
@@ -3357,12 +3357,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3372,34 +3372,34 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F72">
         <v>7</v>
       </c>
       <c r="G72">
-        <v>93.15929966666667</v>
+        <v>295.9323418934911</v>
       </c>
       <c r="H72">
-        <v>11.49691335897437</v>
+        <v>24.19849758211387</v>
       </c>
       <c r="I72">
-        <v>0.0005855445378632366</v>
+        <v>2.136313821045617E-06</v>
       </c>
       <c r="J72">
-        <v>-44.516446</v>
+        <v>-502.82544</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3414,34 +3414,34 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~Time)p(~wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F73">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G73">
-        <v>93.34867718181819</v>
+        <v>295.9623928571428</v>
       </c>
       <c r="H73">
-        <v>11.68629087412589</v>
+        <v>24.22854854576559</v>
       </c>
       <c r="I73">
-        <v>0.000532644110306252</v>
+        <v>2.104454625821533E-06</v>
       </c>
       <c r="J73">
-        <v>-51.84222</v>
+        <v>-504.98981</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3456,39 +3456,39 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~1)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F74">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G74">
-        <v>93.37778056521739</v>
+        <v>296.2407071929825</v>
       </c>
       <c r="H74">
-        <v>11.71539425752509</v>
+        <v>24.50686288160523</v>
       </c>
       <c r="I74">
-        <v>0.0005249493590325164</v>
+        <v>1.831067592307512E-06</v>
       </c>
       <c r="J74">
-        <v>-47.892169</v>
+        <v>-498.20523</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3498,39 +3498,39 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~Time)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F75">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G75">
-        <v>93.40790618181819</v>
+        <v>296.6220776470588</v>
       </c>
       <c r="H75">
-        <v>11.74551987412589</v>
+        <v>24.88823333568155</v>
       </c>
       <c r="I75">
-        <v>0.0005171014019897402</v>
+        <v>1.513180842571757E-06</v>
       </c>
       <c r="J75">
-        <v>-51.782992</v>
+        <v>-499.9671</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3540,39 +3540,39 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~Time)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F76">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G76">
-        <v>93.46747718181818</v>
+        <v>296.8225076470588</v>
       </c>
       <c r="H76">
-        <v>11.80509087412588</v>
+        <v>25.08866333568159</v>
       </c>
       <c r="I76">
-        <v>0.0005019263976188525</v>
+        <v>1.368888303988023E-06</v>
       </c>
       <c r="J76">
-        <v>-51.723421</v>
+        <v>-499.76667</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3582,39 +3582,39 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~temp + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F77">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G77">
-        <v>93.52131018181819</v>
+        <v>296.9414418934912</v>
       </c>
       <c r="H77">
-        <v>11.85892387412589</v>
+        <v>25.20759758211392</v>
       </c>
       <c r="I77">
-        <v>0.0004885964976444136</v>
+        <v>1.289857607207593E-06</v>
       </c>
       <c r="J77">
-        <v>-51.669588</v>
+        <v>-501.81634</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3624,39 +3624,39 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F78">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G78">
-        <v>93.59083556521739</v>
+        <v>296.9628518934912</v>
       </c>
       <c r="H78">
-        <v>11.92844925752509</v>
+        <v>25.22900758211392</v>
       </c>
       <c r="I78">
-        <v>0.0004719033977965852</v>
+        <v>1.276123325424414E-06</v>
       </c>
       <c r="J78">
-        <v>-47.679114</v>
+        <v>-501.79493</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3666,39 +3666,39 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~Time)N(~1)</t>
+          <t>Phi(~1)p(~Time)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F79">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G79">
-        <v>94.15999318181818</v>
+        <v>297.1405318934911</v>
       </c>
       <c r="H79">
-        <v>12.49760687412588</v>
+        <v>25.40668758211388</v>
       </c>
       <c r="I79">
-        <v>0.0003550275849897499</v>
+        <v>1.16764258346799E-06</v>
       </c>
       <c r="J79">
-        <v>-51.030905</v>
+        <v>-501.61725</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3708,39 +3708,39 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + wind + sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F80">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G80">
-        <v>94.25871318181818</v>
+        <v>297.7330928571428</v>
       </c>
       <c r="H80">
-        <v>12.59632687412588</v>
+        <v>25.99924854576557</v>
       </c>
       <c r="I80">
-        <v>0.0003379288906486184</v>
+        <v>8.682343159030933E-07</v>
       </c>
       <c r="J80">
-        <v>-50.932185</v>
+        <v>-503.2191</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3750,23 +3750,23 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~Time)N(~1)</t>
+          <t>Phi(~Time)p(~wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F81">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G81">
-        <v>94.45301518181819</v>
+        <v>297.8213376470588</v>
       </c>
       <c r="H81">
-        <v>12.79062887412589</v>
+        <v>26.08749333568159</v>
       </c>
       <c r="I81">
-        <v>0.0003066430877517954</v>
+        <v>8.307585777332771E-07</v>
       </c>
       <c r="J81">
-        <v>-50.737883</v>
+        <v>-498.76784</v>
       </c>
     </row>
     <row r="82">
@@ -3777,7 +3777,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3792,29 +3792,29 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F82">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G82">
-        <v>94.99911718181819</v>
+        <v>298.1131628571428</v>
       </c>
       <c r="H82">
-        <v>13.33673087412589</v>
+        <v>26.37931854576556</v>
       </c>
       <c r="I82">
-        <v>0.0002333719401917022</v>
+        <v>7.179691685784721E-07</v>
       </c>
       <c r="J82">
-        <v>-50.191781</v>
+        <v>-502.83903</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3824,7 +3824,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3834,39 +3834,39 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~1)p(~temp + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F83">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G83">
-        <v>95.03555118181819</v>
+        <v>299.7600076470588</v>
       </c>
       <c r="H83">
-        <v>13.37316487412589</v>
+        <v>28.02616333568159</v>
       </c>
       <c r="I83">
-        <v>0.0002291590927831813</v>
+        <v>3.151359813401188E-07</v>
       </c>
       <c r="J83">
-        <v>-50.155347</v>
+        <v>-496.82917</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3876,34 +3876,34 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F84">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G84">
-        <v>95.61170647619048</v>
+        <v>299.8737618934912</v>
       </c>
       <c r="H84">
-        <v>13.94932016849818</v>
+        <v>28.13991758211392</v>
       </c>
       <c r="I84">
-        <v>0.0001718013458721739</v>
+        <v>2.977121586830004E-07</v>
       </c>
       <c r="J84">
-        <v>-53.873564</v>
+        <v>-498.88402</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3918,29 +3918,29 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F85">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G85">
-        <v>96.66126418181818</v>
+        <v>301.6237471929825</v>
       </c>
       <c r="H85">
-        <v>14.99887787412588</v>
+        <v>29.88990288160522</v>
       </c>
       <c r="I85">
-        <v>0.0001016524854317122</v>
+        <v>1.241058039573171E-07</v>
       </c>
       <c r="J85">
-        <v>-48.529634</v>
+        <v>-492.82219</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3960,39 +3960,39 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~temp + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F86">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G86">
-        <v>97.09441647619049</v>
+        <v>302.6632876470588</v>
       </c>
       <c r="H86">
-        <v>15.43203016849819</v>
+        <v>30.92944333568158</v>
       </c>
       <c r="I86">
-        <v>8.185782029390275E-05</v>
+        <v>7.380040596482806E-08</v>
       </c>
       <c r="J86">
-        <v>-52.390854</v>
+        <v>-493.92589</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -4002,39 +4002,39 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Phi(~Time)p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~1)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F87">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G87">
-        <v>97.18843147619049</v>
+        <v>308.6874181395349</v>
       </c>
       <c r="H87">
-        <v>15.52604516849819</v>
+        <v>36.95357382815763</v>
       </c>
       <c r="I87">
-        <v>7.809892899246601E-05</v>
+        <v>3.630240814763934E-09</v>
       </c>
       <c r="J87">
-        <v>-52.296839</v>
+        <v>-483.6402</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -4044,39 +4044,39 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F88">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G88">
-        <v>97.19282347619048</v>
+        <v>309.3177771929825</v>
       </c>
       <c r="H88">
-        <v>15.53043716849818</v>
+        <v>37.58393288160522</v>
       </c>
       <c r="I88">
-        <v>7.79276119193918E-05</v>
+        <v>2.648833778393736E-09</v>
       </c>
       <c r="J88">
-        <v>-52.292447</v>
+        <v>-485.12816</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~wind</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -4086,39 +4086,39 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F89">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G89">
-        <v>97.62572547619048</v>
+        <v>310.0744971929824</v>
       </c>
       <c r="H89">
-        <v>15.96333916849818</v>
+        <v>38.34065288160519</v>
       </c>
       <c r="I89">
-        <v>6.276071644727695E-05</v>
+        <v>1.814408391540705E-09</v>
       </c>
       <c r="J89">
-        <v>-51.859545</v>
+        <v>-484.37144</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>~Time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -4128,39 +4128,39 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~Time)N(~1)</t>
+          <t>Phi(~1)p(~sundur + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F90">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G90">
-        <v>98.43271647619048</v>
+        <v>310.5573376470588</v>
       </c>
       <c r="H90">
-        <v>16.77033016849818</v>
+        <v>38.82349333568158</v>
       </c>
       <c r="I90">
-        <v>4.192296818587539E-05</v>
+        <v>1.425238591689294E-09</v>
       </c>
       <c r="J90">
-        <v>-51.052553</v>
+        <v>-486.03183</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>~Time + I(Time^2)</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -4170,23 +4170,23 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
+          <t>Phi(~1)p(~Time)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F91">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G91">
-        <v>101.722346</v>
+        <v>310.9610571929825</v>
       </c>
       <c r="H91">
-        <v>20.0599596923077</v>
+        <v>39.22721288160523</v>
       </c>
       <c r="I91">
-        <v>8.093158551909447E-06</v>
+        <v>1.164718537956986E-09</v>
       </c>
       <c r="J91">
-        <v>-52.486733</v>
+        <v>-483.48488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>